<commit_message>
created functions for file handling
</commit_message>
<xml_diff>
--- a/Student Enrollment Analysis System/scripts/testSplit.xlsx
+++ b/Student Enrollment Analysis System/scripts/testSplit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\CSE303 (Database)\Database-Project\Student Enrollment Analysis System\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2FCA53-BF59-4455-A2C4-C992458485DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C535969-9166-410E-BC02-E6C5A582CA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{20205C2B-4194-462F-B21A-5CC15FE4F85C}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="12450" xr2:uid="{20205C2B-4194-462F-B21A-5CC15FE4F85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>4112-DR Mostafa Kamal</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>FACULTY_FULL_NAME</t>
+  </si>
+  <si>
+    <t>COURSE_NAME</t>
+  </si>
+  <si>
+    <t>Art and Aesthetics</t>
+  </si>
+  <si>
+    <t>Principles of Accounting</t>
+  </si>
+  <si>
+    <t>Management of Accounting</t>
   </si>
 </sst>
 </file>
@@ -423,85 +435,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC1F9FFE-1946-447C-9E0B-D81B036917D6}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.140625" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>